<commit_message>
New forms and edits
</commit_message>
<xml_diff>
--- a/ILRG_ORAM_D_encontros/ILRG_ORAM_D_encontros-media/ILRG_ORAM_D_encontros.xlsx
+++ b/ILRG_ORAM_D_encontros/ILRG_ORAM_D_encontros-media/ILRG_ORAM_D_encontros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\Grants\Dams project\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_D_encontros\ILRG_ORAM_D_encontros-media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\oram\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_D_encontros\ILRG_ORAM_D_encontros-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D4328B-DE37-40A6-92D7-F10D403BD3E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B89238A-C1DF-4B3F-9FD1-A821B7E6105A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="1214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2648" uniqueCount="1216">
   <si>
     <t>type</t>
   </si>
@@ -3730,14 +3730,27 @@
   <si>
     <t>Outro tipo do encontro</t>
   </si>
+  <si>
+    <t>PV040601070</t>
+  </si>
+  <si>
+    <t>Jagarra</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4022,415 +4035,421 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="237">
+  <cellStyleXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="234" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="234" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="236" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="236" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="236" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="236" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="236"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="236"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="237" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="237">
+  <cellStyles count="238">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4668,6 +4687,7 @@
     <cellStyle name="Normal 3 2" xfId="234" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
     <cellStyle name="Normal 3 2 2" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
     <cellStyle name="Normal 3 2 2 2" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Normal 3 2 2 2 3 2" xfId="237" xr:uid="{7D434E13-FE7D-451E-BF4A-FE76E518924A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -5007,7 +5027,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I45" sqref="I45"/>
@@ -5674,7 +5694,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
@@ -6400,9 +6420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G4198"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A519" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C543" sqref="C543"/>
+      <selection pane="bottomLeft" activeCell="C546" sqref="C546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14324,9 +14344,20 @@
       <c r="G539" s="46"/>
     </row>
     <row r="540" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A540" s="42"/>
-      <c r="B540" s="47"/>
-      <c r="C540" s="46"/>
+      <c r="A540" s="85" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B540" s="86" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C540" s="87" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D540" s="86"/>
+      <c r="E540" s="86"/>
+      <c r="F540" s="86" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A541" s="42"/>
@@ -31695,8 +31726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31730,7 +31761,7 @@
         <v>1099</v>
       </c>
       <c r="C2" s="67">
-        <v>201902271</v>
+        <v>201904021</v>
       </c>
       <c r="D2" s="84" t="s">
         <v>1100</v>

</xml_diff>